<commit_message>
Updated test case name as per Jira
</commit_message>
<xml_diff>
--- a/testData/Classification_SC.xlsx
+++ b/testData/Classification_SC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VENKATESHAMKASANAGOT\Documents\MyWorkspace\EADMProject\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5CEB57A-8155-4F25-A2C4-76B8D62F7D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C42F5800-A0B6-4925-8A1C-096C721BF365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -931,7 +931,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1831,7 +1833,7 @@
       <c r="D39" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="E39" s="6" t="s">
         <v>100</v>
       </c>
       <c r="F39" s="7">

</xml_diff>